<commit_message>
-added LJ speech new hyperparam results
</commit_message>
<xml_diff>
--- a/results/ASR-Results.xlsx
+++ b/results/ASR-Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vansh\OneDrive\Documents\GitHub\P4P-Transformer-ASR-for-Dysarthric-Spech\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AAE992-53F7-4F24-A63E-AE289C09D872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FBF4B2-53AF-46AD-8D5F-3B836AF5F068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3528" yWindow="1116" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LJ Speech " sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4524" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4791" uniqueCount="442">
   <si>
     <t>Hyperparameter</t>
   </si>
@@ -835,12 +835,801 @@
   <si>
     <t>Graph Trained on hyperparams above</t>
   </si>
+  <si>
+    <t>LJ Speech new hyperparameters</t>
+  </si>
+  <si>
+    <t>&lt;on the other hand, lords cranworth and wensleydale recommended private executions# so did mr. spencer walpole, m.p.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;on the other hand, and went private executions. so the recommended pay other walkled empe pie and worth exercutions. end a impete,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;in those arguments, quote, and make himself come out top dog, end quote.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;in those artingements, quote, and maken#s, end quote, and maken#s. end quote.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;question# and why was no effort made at that time to inspect his back? answer#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;whese sert made at his back, and while was no effort he init at time to inser.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mrs. tarpey was almost immediately captured and put on her trial, but she was acquitted on the plea that she had acted under the coercion of her husband.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mrs. tarkel, the two her trial, but she had active eagitiently chews almost to meet it was a quitely was almost in the the coorespiar numeront and purbea.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mrs. paine had the actual blanket before her as she testified and she indicated that the blanket hung limp in the officer#s hand.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mrs. paine had the actual blanket of hulebire esheened that been the advice he indicated that the authocia blanket of blanked at hand.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he felt that this was a great man that he had received the letter from, end quote.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;eight the literight man to the litter form, end quote, that he had received a belit head, end quote.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and told him a similar story to craig#s.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and told him a similar strurite to creat strua#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;oswald purchased the money order for the rifle on march twelve, the rifle was shipped on march twenty, and the shooting occurred on april ten.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;oswald purchased the march twenty, and the ship on marchas the money order on march t on april on march as the march as shooting a colok, palasious #the tind.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;this plan will save our national constitution from hardening of the judicial arteries.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;this plan of the gires. are nanwal are per nabause, at from harf per naning of this planiar choseal artries.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;on november twentytwo, oswald told captain fritz that he rode a bus to a stop near his home and then walked to his roominghouse.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;on november twenty to assaled told captain fricze told capss that he rode above  his hold captain frites reminghouse told cates.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;oswald probably engaged his superiors in arguments on a subject that he had studied&gt;</t>
+  </si>
+  <si>
+    <t>&lt;oswald promilately ingates to had he had studied that he had subject he had surperiers in argumants on unasid,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;no additional place would be created.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;no scase would be preated.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;to the exclusion of all other rifles of the same general configuration, end quote.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;to the exclusion of the same jenel conficuration, end quote.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prisoners on reception were treated as they are nowadays  bathed, dressed in prison clothes, and inspected by the surgeon.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prisoners on reception, drescepted as they arm escepted by massepted as they arm the section were treated esurchandles# base#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and i felt like there hadn#t been more than one eyewitness, and if it got to be a known fact that i was an eyewitness, my family or i, either one, might not be safe.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and if ither was an young fact the had one act the eyewitness. mind if theor of which i was an i witness, end no one if it if it if it i hally i witnesse #mi was sayeff.#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and then used the, quote, special treatment, end quote, he received as an example of the way in which he was being picked on and, quote,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and thin youse the way in which he way was, quote, speamet as a next yoused being picked youiled treatment, quote,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he was promptly rescued from his perilous condition, but not before his face and hands were badly scorched.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he was perlasionded from his face and handswerbat photoplation but not phortice courts condition were badly spiral his peraced.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;with atmospheric air containing its ordinary minute dose of carbonic acid and with nothing else but sunlight and heat.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;withat malhing earagent he eat and heat, and with nothing out baried by narry might in heat, and with nothing its ordinary minute,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;when the time is up and the rolls are puffy and promising, set them in a pretty quick oven and bake half an hour,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;when the time in the tyme and bake other, set them as our puffice at the promised out between proteck un the rules and promising and prom a and bain,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;so if i found all of these then i would have been able to say these fibers probably had come from this blanket. but since i found so few,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sit if i would had count of been able the easefied that i wone if been would had count found the sab all of these fires probages thousa.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;whaley was somewhat imprecise as to where he unloaded his passenger.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;whenly was somewhat improse silent his passenger,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;berossus, a priest of the temple of bel at babylon, writing about two fifty b.c.,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;beel at babylong wroch the temple at to fifty southeast of the temple of bebolocis of the temple bell at righting&gt;</t>
+  </si>
+  <si>
+    <t>&lt;these evidences have been in the past thirty years somewhat overshadowed by the far more surprising evidences&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the in the past thirty years somewhat over shat oh dead in the prisons be neved been in the passed been in the past prime of resport sathond,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the costs in heavier debts always doubled the sum# if the arrest was made in the country it trebled it.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the coase was made in the country, if the are wits double this double was made in the country and heavierd debson#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the police wished to refer to greenacre, but as he was not forthcoming,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the police which to referred to greenacre, but as he was not forthor but these were thirt to greenacker,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the exchange of letters dated august thirtyone, nineteen sixtyfour,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the exchanged august thirty of nineteen sixty forid nineteen sixty for.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;through the underpass and leads into an access road,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;through the underpasses roed and leads into and access wore the underpassest and&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and the average daily number committed that year amounted to three thousand, nine hundred eightyfive.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and year amountittip to three thousand, nine hundred eighar are amounted to five remitted thatker three tifth outridier amounting hundred.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;under which wages, hours and working conditions&gt;</t>
+  </si>
+  <si>
+    <t>&lt;under witness, and working conditions wage,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mexico, and was consumed at the rate of a hogshead per week.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mexice head puase a called at the rate of at the rate of uutail,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;was still practiced, that of loading newlyarrived prisoners until they paid certain fees.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;was still they paid#s still they rifle prisoners and that of loading newly arrived, in the paids.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;partisanship, and personal activities on behalf of the cuban government.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;part as inshipp and personal ecubing government#s on be half of the know housemant.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;neighbors and others who knew him at that time recall an introverted boy who read a great deal.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;nabors who new had a great deal red a great aggre it who him at that time while in introver to bory boa.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#i think i could do that sort of job,# said calcraft, on the spur of the moment.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;by calcraft, on the sort of the moment on the speral craft on sent.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and only after the completion of this process can all the food be absorbed into the circulation.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and only after the completion of this process as a circulation of the sourt calcite into the circulation.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;his object in visiting whitchurch was to undermine the honesty of some workman in the mills#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;his object in the mills to one stee of some workman visitor mindles, was to heapten in visitor trials.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;but the vacillating policy in the matter of rudiments does not end here# for it is shown in a still more aggravated form&gt;</t>
+  </si>
+  <si>
+    <t>&lt;but that revacieor for act that vast lating policy in the matter of rodimency in the matter of an her agged form.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;but unlike that of the animal, it is not chiefly an income of foods, but only of the raw materials of food.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;buttle#s of food suffect it is not chiefly animals before #it is not only animal it it is not she fley of the rawn aught bouct,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he had printed a handbill headed in large letters, quote,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he had printed a handbill head in large letters quote,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;this dissection was carried out for newgate prisoners in surgeons# hall, adjoining newgate,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;this that cection was carried out for newgate insert doorning i certions in circe in section was carried outh for knewgate,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;painters, plasterers, and carpenters were allowed to follow their handicrafts, with the reward of sixpence per diem and a double allowance of food.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and and ecrotified. with the reward durs, flaster is a folued. and instrude of six pindelance, with a roans plact of citcepants of followed.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#in our late visits,# they say, #we have seen manifest indications of a retrograde movement in this respect,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;in our late visits respect, reight our let ins they seen manifess in this its indications of erect weat visit.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;frazier doubted whether the bag that oswald carried was as wide as the bag found on the sixth floor, although mrs. randle testified&gt;</t>
+  </si>
+  <si>
+    <t>&lt;frazier down the sixth floor, was as whether the begger day whethouth loor found on the sixth floor, found on the sixth floor.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;but a long public discussion followed, and in consequence he was reprieved.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;but elong public descosion followed. he was reprevieved. and in consequence&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he asked his wife to help him to hijack an airplane to get there, but gave up that scheme when she refused.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he asked do high gave up that skeen when she refused. but nerarplaned to him to get there plane to hhhhelp that their play to,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and that from the time of his conviction nothing but what is consolatory should be addressed to a criminal.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and that from the tyme of his conviction salutory should be antered that from the tyme of his could solictory&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and the curtailment of rank stock speculation through the securities exchange act.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and the courty stocks schael aged by the cab right such stop accuration of rapes stable of #rake#s throught&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the shameful malpractices of bambridge,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the shame full moutery a general practices of babylon briggge.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;that he had sought and obtained a passport on june twentyfive, nineteen sixtythree.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;that he had saw an abterty three thing a passpord on june twenty three.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he had been led to suppose that twelve months# imprisonment was the utmost the law could inflict, and he broke down utterly under the unexpected blow.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he had been lead, and expected blow could in flaw that twelve months apposed the law down to supped and exmocint was the unexpected blaw,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;she said, quote, no# by golly, he didn#t, end quote, and turned around, but the man was nowhere in sight.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;she said quote, no, by gold, end quote, ut the man was no, but and turned round. end quote.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;all this does seem to amount to enough to have induced an alert agency, such as the fbi,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;all this does the fbi, such as the fbi, to have induced an all is enalized anilor egency&gt;</t>
+  </si>
+  <si>
+    <t>&lt;if oswald left the depository building at twelve#thirtythree p.m.,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;if if #if the depository building it well the left oswald left three p.m.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the interesting thing, or rather the danger involved, was the fact that oswald seemed like such a nice, bright boy&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the injureant knice bright such and nine or was the ficting sure involved, was the fict boy that oswald#s bright seemed theying.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;this block contained one hundred and thirty cells, embracing every modern improvement#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;this block contained one hundred in thirty singe heave remodary mars. imbribed.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;they had vacated their apartment, and marina oswald had departed with their child in a station wagon with texas registration.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;they had vaited their aparting with their cise which  tragest registation wagon and marina oswald had department, and vaited their part in a station.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;nor was there any indication that the lift had been performed.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;nor was there any a case inthat the lived had been preformed.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the ink was barely dry upon their letters of appointment before they appeared at newgate, and commenced a searching investigation.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the appeared at newgate, and came investigation, before they perso surching in their letters of a pwhile sertioner, extigation.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;because of insufficient postage, which apparently resulted from an increase in postal rates of which his wife had been unaware.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;because if in sufficient posted #on a ware are where this wife had been enassing of which a parrily result rades in posted in the post deter.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;nor is this goal served when agents remain out until early morning hours, and lose the opportunity to get a reasonable amount of sleep.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;no ordinate instrimals searor is enable amount of soorce, when a generasie to genery#s new morning out to a sear of deters, and loosely ward.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;marina oswald#s testimony indicates that her husband was not particularly concerned about his continued possession of the most incriminating sort of evidence.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;marina oswald in criminating so testimatic possess that his continued possession of the most incriminating concession about his continue concerned about putince,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and measures taken to arrest them when their plans were so far developed that no doubt could remain as to their guilt.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and measures that no day hid no dial a when their plans were so fard of them when their pula take hit to eremate to their could.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;it was thought that this would guarantee constant supervision and inspection, but it did nothing of the kind, and only the presence of warders on duty&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the presence with the presence of warders, on duty arteed with he constance of raranted so to gar, and lastle# at this would do that the examelly, thexe,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the sufferer was a porter on the london, chatham, and dover railway, sentenced to death for shooting the stationmaster at dover.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the suffocient master addrow railwan and does of hort was a porth of rewatch half the rial negae such am the lundon stidon, shooting the stationment addover.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the precious metal was sent from place to place carefully locked up and guarded, no doubt#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the pressus has metal was sent from place carefully locked up and gown doubt,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tippit stopped the man and called him to his car.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tippits topine and car.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;after this nothing remained but to wait for some occasion when the amount transmitted would be sufficient to justify the risks of robbery.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;after this nothing remaind but to weithing rest the transmitt to gent would be sufficient would be seemad would the immoting would be soing bess.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;answer# i said it would be better if i remained with ruth until the holidays, he would come, and we would all meet together.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;answer# i said would all neat bed a would all the home, and maint with he would author, i said ather.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;its bricks, measuring about thirteen inches square and three inches in thickness, were burned and stamped with the usual short inscription#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;its tection were burned inscription with the use who hare and three inches frites in three inches east briterance square end in steam.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;but it was based upon more extended and audacious forgeries.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;but it which stend unmorice forgeries it was vasita pun more extended and oddrereas.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;which grows as one speaks to him, end quote.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;which grose as once key him and quote.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;finally, the entry of january four to thirtyone of nineteen sixtyone, quote,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;finlil eaphind he wonn of ninewery thirty one, #the entry four to thirty one, poort,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;chapter four. the assassin# part five.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;it was so used for the date of the abolition of the star chamber in the sixteenth charles the first&gt;</t>
+  </si>
+  <si>
+    <t>&lt;in the sixteen the abolition of the abolition of the used for charles of eugorized start in the stort of the date.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;in eighteen thirtyseven the death penalty was practically limited to murder or attempts to murder,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;in eighteen forty sabin the defact occe the reteclimate to murder or ten or attempts to murder the sabonip#s emurder,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;solomons also established a system of provincial agency, by which stolen goods were passed on from london to the seaports, and so abroad.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;so established decision goods also into the separate sistone from long goods and so agoon to the seop reving to the seipworcs, and so its done from loom pasters,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;as discussed in chapter six, she failed to report this to agent hosty&gt;</t>
+  </si>
+  <si>
+    <t>&lt;as discussed in chapter or this to agent hosty, she failed to report this to lage inth hunch,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the prison was a nest of abuses, like its neighbor the king#s bench&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the prison was an necednabiage. like it fingestive of a buses, weiton was andi ber&gt;</t>
+  </si>
+  <si>
+    <t>&lt;but in babylonia stone was difficult to obtain, and sculptures were very rare.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;but stoney a long was difficult to exholetory rarius stoniua and scane,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;above the murmur and tumult of that noisy assembly, the lowing and bleating of cattle as they were driven into the stalls and pens of smithfield&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a but to mulds of the mermerusrance smith be of capiled the loys of the stall, as they were driven into the stall, the late entoicinal and bleed to molete asisial&gt;</t>
+  </si>
+  <si>
+    <t>&lt;as in a mountainous country, it is impossible to say where mountain ends and valley begins# as in the development of an animal,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;as it is empossible to say, whare mount in ensenable to in ens and valed its emont in the divelt addisonist continet animal.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;why not relieve newgate by drawing more largely upon the superior accommodation which millbank offered?&gt;</t>
+  </si>
+  <si>
+    <t>&lt;while not relargely appoint, newgate, by nation which nill be vil beder commodation which lange newgate,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mr. newman admitted that he had petitioned that certain #trusty men# might be left in the jail.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mr. newmen, that he had petitioned that ste might the left in the jail man admitted to shine that certoon in it it admeaill.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;whatever their purposes presidential journeys have greatly enlarged and complicated the task of protecting the president.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#what her persident and girge, and complicated the task of protecting the president.# protecting the president.# protecting the president.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;police sirens sounded along jefferson boulevard.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;police sirens blonge jefeth of a sen boelthard.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;all vertebrates, and none other, have a number of their anterior vertebral joints enlarged and consolidated into a box to form the skull,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;all verter direts, and cherious # have a adotayry a verter a been unator hopel, and unon autorited had nother and he scalled joyer retched and hir her her.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;advance preparations.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;edpans preparations.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;under our system of justice no forum could properly make that determination unless oswald were before it.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;under oscistian at a to have justices no form of gest oswald work work worth dusticess oswald work that #t.#.#.#.#c.#.#o.#e.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;his marine career was not helped by his attitude&gt;</t>
+  </si>
+  <si>
+    <t>&lt;his marine correor was not healt by his at a tudde&gt;</t>
+  </si>
+  <si>
+    <t>&lt;for while roman catholics and dissenters were encouraged to see ministers of their own persuasion,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;for one procedemen carrong catlain for our roman catlain for while recenters of their own preceden&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#do tell me, sir# i am informed i shall go down with great force# is it so?#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;down with greatful, i am it for dr. greatf arment brick four a seas.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;in the plant also oxygen is absorbed through the epidermis and stomata from the air.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;in the plant oxygen as emoxyger mr. whalked up from the eart through the iremod from the ear.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he wanted a light for a cigar, and got it from a lantern which was lifted up and fully betrayed his features.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he betrom a light from a lanter assigar no llanted others, and got it was lifeates with a life fully betrom which was.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the vice president conferred with white house assistant press secretary malcolm kilduff&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the vice president confirm culloficys is to president could fild off.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;oswald#s departure from building.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;oswald#s the parturford from building.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;in evaluating data processing techniques of the secret service,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;in evaluating day sourt secaris and the secret service,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;with the alinement of the assassin#s rifle, at a range of one hundred seventyseven to two hundred sixtysix feet.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;with the allined and excevine to two under seven to six of the assassin#s rifle, age of one hundred seven to ted sixty six feet.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;to be able to provide effective continuing supervision&gt;</t>
+  </si>
+  <si>
+    <t>&lt;to be in o#t of continual to provide effective continued#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a heavy brutish fellow, was yet aghast at his wife#s resolve, and tried hard to dissuade her from bad purpose.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a have gatered to disway heard to desway her from badach fold and trifce resulate his wife# was yet again hard to disway and tried her felow tha&gt;</t>
+  </si>
+  <si>
+    <t>&lt;on october three, hosty reopened the case in dallas to assist the new orleans office.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;on october three opposed to has siste the new orleans officence in dallas office.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;well, in order to achieve three hits, it would not be required that a man be an exceptional shot. a proficient man with this weapon, yes, end quote.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;wheleen order that a man with three hinan appense, et while in order than be an exhites, appain, end quote, a perfection man where three required this, we.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;but in either event he would have been in the roominghouse at about one p.m.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;but an i.thern p. he would have been in the roominghouse at a gone p.m. doeop one p. huld house and i.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the chronicles of newgate, volume two. by arthur griffiths. section thirteen# newgate notorieties, part one.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the conner wills of newgate, volume two. by arthur t. nunighteen, notorieties, section thirteen, newgate note aithes part one.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;when such goods arrived they were frequently left at a wharf, paying rent until it suited the importer to remove them.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;when suid# went frequently left at ab paine arrent to remove the importer to good the were frequer to work frequently left guid#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;where within the limits of the same natural group of organisms a rudiment is sometimes present and sometimes absent.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;whare within the limits of the same is and some time its own time its some time its and the limits of the same belong besent.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;national laws are needed to complete that program.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;national laws are need that probrab,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the employees raced the elevators to the first floor. givens saw oswald standing at the gate on the fifth floor as the elevator went by.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the elevator when the floor as the elevator suw of eight on the fifth floor as the elevator standing at the gater went nequired by as the even soft floor.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;it was benavides, using tippit#s car radio, who first reported the killing of patrolman tippit at about one#sixteen p.m.#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;it was beneviewd the killing of partipat# at about who first report for scarrried the killing who first he eas, who had been to had the carrrawb,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;onto the rear of the presidential plane where seats had been removed to make room.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;on to the receited had been remained were seet had been removed to make rooom.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he adhered to this almost to the very last. his case had been warmly espoused by the society for the protection of germans in this country,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he adeked this case had been warman#s in this almost by the spound trade to the very labsoled to the very techn been wormands on traadi he for the protection of jurmmons#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;they intentionally mentioned a most unfavorable hour.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;they intentiond did unfavor of eighteen tentionaly mentionded unthraugh urble hour.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;called the clerk of the papers, attends daily. end quote.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;callerk of the papers attend utilit of the clork of the papers attand you.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;their main function was to spot trouble in advance and to direct any necessary steps to meet the trouble.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;there may necessary spotted any necessary service to meet the truble in advance assoct any necessary spotrache.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;for cyrus had done neither the one nor the other when he took babylon.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;for sight the the wanth babylon, nor the one he took nor the one.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;who yet faced extraordinary risks to advance their enlargement by only a few hours.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;who it vansed their largemen by only a few hours, to a drisk faced extraduous.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the first constable who entered thistlewood ran through the body with a sword, but others quickly followed,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;these awaitard through the body with a sorred, but others quickly first constable would, and turd #the fibed##&gt;</t>
+  </si>
+  <si>
+    <t>&lt;which advise it of potential threats immediately before the visit of the president to their community.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;which adappeasaded before the visit of the president to their community before the businety.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the fireside chats of franklin delano roosevelt, by franklin d roosevelt, section six.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;the fireside chapsian six indellined by rose vive frige when deline ose of bibe franklened rousevelt,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prescribed nominally by the fresh doctor, for which palmer had substituted his own.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;parsured had substituded his ownly by the fresh palmer for  high had substituded his own.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;vicepresidential car.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;vice presidential car.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he seems to have improved the occasion when preaching the condemned sermon before fauntleroy, by pointing a moral from that unhappy man#s own case.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he seems to have a been a mans own casion went in when prejument cermon happing the condemned cermon happing a case in immarine precinemnened sermon before funs.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he carried me away by fraud and stratagem, and forced me to accompany him to gretna green&gt;</t>
+  </si>
+  <si>
+    <t>&lt;he carpenied to great neighborhand and forcina way meale a couple couple accopcant gimmial way him.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and the costliness of enlarging it, forbade all idea of entirely reconstructing the jail so as to constitute it a model prison.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;and the constling ele so as to constitute all slingestly recounstliness of interrion the jail, for bail, so as to cyoung largely at,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;these were undoubtedly perennibranchs. in the permian and triassic higher forms appeared, which were certainly caducibranch.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;these regad downs appeared which wourse ppeared in a brought high as wrinly caducially in tryas higher forms abork.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;that the interruption shall not take place for an hour, end quote.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;that the interrouchined, quote, #end quote, own not take place for an all reque.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;in another borough, with a population of ten thousand, the prison was of the same dimensions.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;in another burrero opened amengion of the same dimention of the same did mention sayings.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;so far as the fbi knew he had not shown any potential for violence.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;so the farras the filed reviolence, he had not shown anytheres the so forbi anyther is.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a space of about twentythree feet separated it from its inner part, which was about twenty feet in width.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a separated through the inner part when the chrommits of about twenty feet in wide the feat separated it washeteadory from ited thirty it cart hitkead ce wing.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;they are absorbed by the circulating liquids and carried to the eliminating organs, lungs and kidneys chiefly, for elimination.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;there irea ealliminating organ by the city, for ellecting liquotes, and carried to the elictit the aliminating organ diminating or obsord long exordeed.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;which gave him access to all parts of the mills, the packingroom included.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;which gave him accis, the packing room included, the magust of the packing rooming cases the all partses,&gt;</t>
+  </si>
+  <si>
+    <t>&lt;they talked of the days when the convicts were hung up a dozen or more in a row#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;they talk dousnoner more in a rope under the duss and the convicts were home accompanic swere.&gt;</t>
+  </si>
+  <si>
+    <t>New hyperparam results</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -886,6 +1675,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -922,7 +1717,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -936,6 +1731,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -990,6 +1789,50 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
+          <a:ext cx="6095238" cy="4571429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>608838</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>182309</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C0EF346-DBDD-B831-23CE-33D631FA59DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5120640"/>
           <a:ext cx="6095238" cy="4571429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1380,15 +2223,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:W132"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="19" max="19" width="14.6640625" customWidth="1"/>
+    <col min="21" max="21" width="20.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1398,45 +2245,1496 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S1" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="L2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="U2" t="s">
+        <v>180</v>
+      </c>
+      <c r="V2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="L3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="U3" t="s">
+        <v>182</v>
+      </c>
+      <c r="V3" t="s">
+        <v>183</v>
+      </c>
+      <c r="W3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="L4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="U4" t="s">
+        <v>184</v>
+      </c>
+      <c r="V4" t="s">
+        <v>185</v>
+      </c>
+      <c r="W4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="L5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="U5" t="s">
+        <v>186</v>
+      </c>
+      <c r="V5" t="s">
+        <v>187</v>
+      </c>
+      <c r="W5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="L6" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="U6" t="s">
+        <v>188</v>
+      </c>
+      <c r="V6" t="s">
+        <v>189</v>
+      </c>
+      <c r="W6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="L7" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="U7" t="s">
+        <v>190</v>
+      </c>
+      <c r="V7" t="s">
+        <v>191</v>
+      </c>
+      <c r="W7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="L8" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="U8" t="s">
+        <v>192</v>
+      </c>
+      <c r="V8" t="s">
+        <v>193</v>
+      </c>
+      <c r="W8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U9" t="s">
+        <v>194</v>
+      </c>
+      <c r="V9" t="s">
+        <v>195</v>
+      </c>
+      <c r="W9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U10" t="s">
+        <v>196</v>
+      </c>
+      <c r="V10" t="s">
+        <v>197</v>
+      </c>
+      <c r="W10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U11" t="s">
+        <v>198</v>
+      </c>
+      <c r="V11" t="s">
+        <v>199</v>
+      </c>
+      <c r="W11">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U12" t="s">
+        <v>200</v>
+      </c>
+      <c r="V12" t="s">
+        <v>201</v>
+      </c>
+      <c r="W12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U13" t="s">
+        <v>202</v>
+      </c>
+      <c r="V13" t="s">
+        <v>203</v>
+      </c>
+      <c r="W13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U14" t="s">
+        <v>204</v>
+      </c>
+      <c r="V14" t="s">
+        <v>205</v>
+      </c>
+      <c r="W14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U15" t="s">
+        <v>206</v>
+      </c>
+      <c r="V15" t="s">
+        <v>207</v>
+      </c>
+      <c r="W15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U16" t="s">
+        <v>208</v>
+      </c>
+      <c r="V16" t="s">
+        <v>209</v>
+      </c>
+      <c r="W16">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U17" t="s">
+        <v>210</v>
+      </c>
+      <c r="V17" t="s">
+        <v>211</v>
+      </c>
+      <c r="W17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U18" t="s">
+        <v>212</v>
+      </c>
+      <c r="V18" t="s">
+        <v>213</v>
+      </c>
+      <c r="W18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U19" t="s">
+        <v>214</v>
+      </c>
+      <c r="V19" t="s">
+        <v>215</v>
+      </c>
+      <c r="W19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U20" t="s">
+        <v>216</v>
+      </c>
+      <c r="V20" t="s">
+        <v>217</v>
+      </c>
+      <c r="W20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U21" t="s">
+        <v>218</v>
+      </c>
+      <c r="V21" t="s">
+        <v>219</v>
+      </c>
+      <c r="W21">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U22" t="s">
+        <v>220</v>
+      </c>
+      <c r="V22" t="s">
+        <v>221</v>
+      </c>
+      <c r="W22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U23" t="s">
+        <v>222</v>
+      </c>
+      <c r="V23" t="s">
+        <v>223</v>
+      </c>
+      <c r="W23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U24" t="s">
+        <v>224</v>
+      </c>
+      <c r="V24" t="s">
+        <v>225</v>
+      </c>
+      <c r="W24">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U25" t="s">
+        <v>226</v>
+      </c>
+      <c r="V25" t="s">
+        <v>227</v>
+      </c>
+      <c r="W25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U26" t="s">
+        <v>228</v>
+      </c>
+      <c r="V26" t="s">
+        <v>229</v>
+      </c>
+      <c r="W26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="U27" t="s">
+        <v>230</v>
+      </c>
+      <c r="V27" t="s">
+        <v>231</v>
+      </c>
+      <c r="W27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U28" t="s">
+        <v>232</v>
+      </c>
+      <c r="V28" t="s">
+        <v>233</v>
+      </c>
+      <c r="W28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U29" t="s">
+        <v>234</v>
+      </c>
+      <c r="V29" t="s">
+        <v>235</v>
+      </c>
+      <c r="W29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U30" t="s">
+        <v>236</v>
+      </c>
+      <c r="V30" t="s">
+        <v>237</v>
+      </c>
+      <c r="W30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U31" t="s">
+        <v>238</v>
+      </c>
+      <c r="V31" t="s">
+        <v>239</v>
+      </c>
+      <c r="W31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U32" t="s">
+        <v>240</v>
+      </c>
+      <c r="V32" t="s">
+        <v>241</v>
+      </c>
+      <c r="W32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U33" t="s">
+        <v>242</v>
+      </c>
+      <c r="V33" t="s">
+        <v>243</v>
+      </c>
+      <c r="W33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U34" t="s">
+        <v>244</v>
+      </c>
+      <c r="V34" t="s">
+        <v>245</v>
+      </c>
+      <c r="W34">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U35" t="s">
+        <v>246</v>
+      </c>
+      <c r="V35" t="s">
+        <v>247</v>
+      </c>
+      <c r="W35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U36" t="s">
+        <v>248</v>
+      </c>
+      <c r="V36" t="s">
+        <v>249</v>
+      </c>
+      <c r="W36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U37" t="s">
+        <v>250</v>
+      </c>
+      <c r="V37" t="s">
+        <v>251</v>
+      </c>
+      <c r="W37">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U38" t="s">
+        <v>252</v>
+      </c>
+      <c r="V38" t="s">
+        <v>253</v>
+      </c>
+      <c r="W38">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U39" t="s">
+        <v>254</v>
+      </c>
+      <c r="V39" t="s">
+        <v>255</v>
+      </c>
+      <c r="W39">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U40" t="s">
+        <v>256</v>
+      </c>
+      <c r="V40" t="s">
+        <v>257</v>
+      </c>
+      <c r="W40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U41" t="s">
+        <v>258</v>
+      </c>
+      <c r="V41" t="s">
+        <v>259</v>
+      </c>
+      <c r="W41">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U42" t="s">
+        <v>260</v>
+      </c>
+      <c r="V42" t="s">
+        <v>261</v>
+      </c>
+      <c r="W42">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U43" t="s">
+        <v>262</v>
+      </c>
+      <c r="V43" t="s">
+        <v>263</v>
+      </c>
+      <c r="W43">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U44" t="s">
+        <v>264</v>
+      </c>
+      <c r="V44" t="s">
+        <v>265</v>
+      </c>
+      <c r="W44">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U45" t="s">
+        <v>266</v>
+      </c>
+      <c r="V45" t="s">
+        <v>267</v>
+      </c>
+      <c r="W45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U46" t="s">
+        <v>268</v>
+      </c>
+      <c r="V46" t="s">
+        <v>269</v>
+      </c>
+      <c r="W46">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U47" t="s">
+        <v>270</v>
+      </c>
+      <c r="V47" t="s">
+        <v>271</v>
+      </c>
+      <c r="W47">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U48" t="s">
+        <v>272</v>
+      </c>
+      <c r="V48" t="s">
+        <v>273</v>
+      </c>
+      <c r="W48">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U49" t="s">
+        <v>274</v>
+      </c>
+      <c r="V49" t="s">
+        <v>275</v>
+      </c>
+      <c r="W49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U50" t="s">
+        <v>276</v>
+      </c>
+      <c r="V50" t="s">
+        <v>277</v>
+      </c>
+      <c r="W50">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U51" t="s">
+        <v>278</v>
+      </c>
+      <c r="V51" t="s">
+        <v>279</v>
+      </c>
+      <c r="W51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U52" t="s">
+        <v>280</v>
+      </c>
+      <c r="V52" t="s">
+        <v>281</v>
+      </c>
+      <c r="W52">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U53" t="s">
+        <v>282</v>
+      </c>
+      <c r="V53" t="s">
+        <v>283</v>
+      </c>
+      <c r="W53">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U54" t="s">
+        <v>284</v>
+      </c>
+      <c r="V54" t="s">
+        <v>285</v>
+      </c>
+      <c r="W54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U55" t="s">
+        <v>286</v>
+      </c>
+      <c r="V55" t="s">
+        <v>287</v>
+      </c>
+      <c r="W55">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U56" t="s">
+        <v>288</v>
+      </c>
+      <c r="V56" t="s">
+        <v>289</v>
+      </c>
+      <c r="W56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U57" t="s">
+        <v>290</v>
+      </c>
+      <c r="V57" t="s">
+        <v>291</v>
+      </c>
+      <c r="W57">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U58" t="s">
+        <v>292</v>
+      </c>
+      <c r="V58" t="s">
+        <v>293</v>
+      </c>
+      <c r="W58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U59" t="s">
+        <v>294</v>
+      </c>
+      <c r="V59" t="s">
+        <v>295</v>
+      </c>
+      <c r="W59">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U60" t="s">
+        <v>296</v>
+      </c>
+      <c r="V60" t="s">
+        <v>297</v>
+      </c>
+      <c r="W60">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U61" t="s">
+        <v>298</v>
+      </c>
+      <c r="V61" t="s">
+        <v>299</v>
+      </c>
+      <c r="W61">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U62" t="s">
+        <v>300</v>
+      </c>
+      <c r="V62" t="s">
+        <v>301</v>
+      </c>
+      <c r="W62">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U63" t="s">
+        <v>302</v>
+      </c>
+      <c r="V63" t="s">
+        <v>303</v>
+      </c>
+      <c r="W63">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U64" t="s">
+        <v>304</v>
+      </c>
+      <c r="V64" t="s">
+        <v>305</v>
+      </c>
+      <c r="W64">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U65" t="s">
+        <v>306</v>
+      </c>
+      <c r="V65" t="s">
+        <v>307</v>
+      </c>
+      <c r="W65">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U66" t="s">
+        <v>308</v>
+      </c>
+      <c r="V66" t="s">
+        <v>309</v>
+      </c>
+      <c r="W66">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U67" t="s">
+        <v>310</v>
+      </c>
+      <c r="V67" t="s">
+        <v>311</v>
+      </c>
+      <c r="W67">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U68" t="s">
+        <v>312</v>
+      </c>
+      <c r="V68" t="s">
+        <v>313</v>
+      </c>
+      <c r="W68">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U69" t="s">
+        <v>314</v>
+      </c>
+      <c r="V69" t="s">
+        <v>315</v>
+      </c>
+      <c r="W69">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U70" t="s">
+        <v>316</v>
+      </c>
+      <c r="V70" t="s">
+        <v>317</v>
+      </c>
+      <c r="W70">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U71" t="s">
+        <v>318</v>
+      </c>
+      <c r="V71" t="s">
+        <v>319</v>
+      </c>
+      <c r="W71">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U72" t="s">
+        <v>320</v>
+      </c>
+      <c r="V72" t="s">
+        <v>321</v>
+      </c>
+      <c r="W72">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U73" t="s">
+        <v>322</v>
+      </c>
+      <c r="V73" t="s">
+        <v>323</v>
+      </c>
+      <c r="W73">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U74" t="s">
+        <v>324</v>
+      </c>
+      <c r="V74" t="s">
+        <v>324</v>
+      </c>
+      <c r="W74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U75" t="s">
+        <v>325</v>
+      </c>
+      <c r="V75" t="s">
+        <v>326</v>
+      </c>
+      <c r="W75">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U76" t="s">
+        <v>327</v>
+      </c>
+      <c r="V76" t="s">
+        <v>328</v>
+      </c>
+      <c r="W76">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U77" t="s">
+        <v>329</v>
+      </c>
+      <c r="V77" t="s">
+        <v>330</v>
+      </c>
+      <c r="W77">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U78" t="s">
+        <v>331</v>
+      </c>
+      <c r="V78" t="s">
+        <v>332</v>
+      </c>
+      <c r="W78">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U79" t="s">
+        <v>333</v>
+      </c>
+      <c r="V79" t="s">
+        <v>334</v>
+      </c>
+      <c r="W79">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U80" t="s">
+        <v>335</v>
+      </c>
+      <c r="V80" t="s">
+        <v>336</v>
+      </c>
+      <c r="W80">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U81" t="s">
+        <v>337</v>
+      </c>
+      <c r="V81" t="s">
+        <v>338</v>
+      </c>
+      <c r="W81">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="82" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U82" t="s">
+        <v>339</v>
+      </c>
+      <c r="V82" t="s">
+        <v>340</v>
+      </c>
+      <c r="W82">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U83" t="s">
+        <v>341</v>
+      </c>
+      <c r="V83" t="s">
+        <v>342</v>
+      </c>
+      <c r="W83">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U84" t="s">
+        <v>343</v>
+      </c>
+      <c r="V84" t="s">
+        <v>344</v>
+      </c>
+      <c r="W84">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U85" t="s">
+        <v>345</v>
+      </c>
+      <c r="V85" t="s">
+        <v>346</v>
+      </c>
+      <c r="W85">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U86" t="s">
+        <v>347</v>
+      </c>
+      <c r="V86" t="s">
+        <v>348</v>
+      </c>
+      <c r="W86">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U87" t="s">
+        <v>349</v>
+      </c>
+      <c r="V87" t="s">
+        <v>350</v>
+      </c>
+      <c r="W87">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U88" t="s">
+        <v>351</v>
+      </c>
+      <c r="V88" t="s">
+        <v>352</v>
+      </c>
+      <c r="W88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U89" t="s">
+        <v>353</v>
+      </c>
+      <c r="V89" t="s">
+        <v>354</v>
+      </c>
+      <c r="W89">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="90" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U90" t="s">
+        <v>355</v>
+      </c>
+      <c r="V90" t="s">
+        <v>356</v>
+      </c>
+      <c r="W90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U91" t="s">
+        <v>357</v>
+      </c>
+      <c r="V91" t="s">
+        <v>358</v>
+      </c>
+      <c r="W91">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U92" t="s">
+        <v>359</v>
+      </c>
+      <c r="V92" t="s">
+        <v>360</v>
+      </c>
+      <c r="W92">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U93" t="s">
+        <v>361</v>
+      </c>
+      <c r="V93" t="s">
+        <v>362</v>
+      </c>
+      <c r="W93">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U94" t="s">
+        <v>363</v>
+      </c>
+      <c r="V94" t="s">
+        <v>364</v>
+      </c>
+      <c r="W94">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U95" t="s">
+        <v>365</v>
+      </c>
+      <c r="V95" t="s">
+        <v>366</v>
+      </c>
+      <c r="W95">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U96" t="s">
+        <v>367</v>
+      </c>
+      <c r="V96" t="s">
+        <v>368</v>
+      </c>
+      <c r="W96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U97" t="s">
+        <v>369</v>
+      </c>
+      <c r="V97" t="s">
+        <v>370</v>
+      </c>
+      <c r="W97">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U98" t="s">
+        <v>371</v>
+      </c>
+      <c r="V98" t="s">
+        <v>372</v>
+      </c>
+      <c r="W98">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="99" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U99" t="s">
+        <v>373</v>
+      </c>
+      <c r="V99" t="s">
+        <v>374</v>
+      </c>
+      <c r="W99">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U100" t="s">
+        <v>375</v>
+      </c>
+      <c r="V100" t="s">
+        <v>376</v>
+      </c>
+      <c r="W100">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="101" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U101" t="s">
+        <v>377</v>
+      </c>
+      <c r="V101" t="s">
+        <v>378</v>
+      </c>
+      <c r="W101">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U102" t="s">
+        <v>379</v>
+      </c>
+      <c r="V102" t="s">
+        <v>380</v>
+      </c>
+      <c r="W102">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="103" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U103" t="s">
+        <v>381</v>
+      </c>
+      <c r="V103" t="s">
+        <v>382</v>
+      </c>
+      <c r="W103">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U104" t="s">
+        <v>383</v>
+      </c>
+      <c r="V104" t="s">
+        <v>384</v>
+      </c>
+      <c r="W104">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U105" t="s">
+        <v>385</v>
+      </c>
+      <c r="V105" t="s">
+        <v>386</v>
+      </c>
+      <c r="W105">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U106" t="s">
+        <v>387</v>
+      </c>
+      <c r="V106" t="s">
+        <v>388</v>
+      </c>
+      <c r="W106">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="107" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U107" t="s">
+        <v>389</v>
+      </c>
+      <c r="V107" t="s">
+        <v>390</v>
+      </c>
+      <c r="W107">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U108" t="s">
+        <v>391</v>
+      </c>
+      <c r="V108" t="s">
+        <v>392</v>
+      </c>
+      <c r="W108">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="109" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U109" t="s">
+        <v>393</v>
+      </c>
+      <c r="V109" t="s">
+        <v>394</v>
+      </c>
+      <c r="W109">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="110" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U110" t="s">
+        <v>395</v>
+      </c>
+      <c r="V110" t="s">
+        <v>396</v>
+      </c>
+      <c r="W110">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U111" t="s">
+        <v>397</v>
+      </c>
+      <c r="V111" t="s">
+        <v>398</v>
+      </c>
+      <c r="W111">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="112" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U112" t="s">
+        <v>399</v>
+      </c>
+      <c r="V112" t="s">
+        <v>400</v>
+      </c>
+      <c r="W112">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U113" t="s">
+        <v>401</v>
+      </c>
+      <c r="V113" t="s">
+        <v>402</v>
+      </c>
+      <c r="W113">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U114" t="s">
+        <v>403</v>
+      </c>
+      <c r="V114" t="s">
+        <v>404</v>
+      </c>
+      <c r="W114">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="115" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U115" t="s">
+        <v>405</v>
+      </c>
+      <c r="V115" t="s">
+        <v>406</v>
+      </c>
+      <c r="W115">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U116" t="s">
+        <v>407</v>
+      </c>
+      <c r="V116" t="s">
+        <v>408</v>
+      </c>
+      <c r="W116">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="117" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U117" t="s">
+        <v>409</v>
+      </c>
+      <c r="V117" t="s">
+        <v>410</v>
+      </c>
+      <c r="W117">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="118" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U118" t="s">
+        <v>411</v>
+      </c>
+      <c r="V118" t="s">
+        <v>412</v>
+      </c>
+      <c r="W118">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U119" t="s">
+        <v>413</v>
+      </c>
+      <c r="V119" t="s">
+        <v>414</v>
+      </c>
+      <c r="W119">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U120" t="s">
+        <v>415</v>
+      </c>
+      <c r="V120" t="s">
+        <v>416</v>
+      </c>
+      <c r="W120">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U121" t="s">
+        <v>417</v>
+      </c>
+      <c r="V121" t="s">
+        <v>418</v>
+      </c>
+      <c r="W121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U122" t="s">
+        <v>419</v>
+      </c>
+      <c r="V122" t="s">
+        <v>420</v>
+      </c>
+      <c r="W122">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="123" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U123" t="s">
+        <v>421</v>
+      </c>
+      <c r="V123" t="s">
+        <v>422</v>
+      </c>
+      <c r="W123">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="124" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U124" t="s">
+        <v>423</v>
+      </c>
+      <c r="V124" t="s">
+        <v>424</v>
+      </c>
+      <c r="W124">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="125" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U125" t="s">
+        <v>425</v>
+      </c>
+      <c r="V125" t="s">
+        <v>426</v>
+      </c>
+      <c r="W125">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="126" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U126" t="s">
+        <v>427</v>
+      </c>
+      <c r="V126" t="s">
+        <v>428</v>
+      </c>
+      <c r="W126">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U127" t="s">
+        <v>429</v>
+      </c>
+      <c r="V127" t="s">
+        <v>430</v>
+      </c>
+      <c r="W127">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U128" t="s">
+        <v>431</v>
+      </c>
+      <c r="V128" t="s">
+        <v>432</v>
+      </c>
+      <c r="W128">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U129" t="s">
+        <v>433</v>
+      </c>
+      <c r="V129" t="s">
+        <v>434</v>
+      </c>
+      <c r="W129">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="130" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U130" t="s">
+        <v>435</v>
+      </c>
+      <c r="V130" t="s">
+        <v>436</v>
+      </c>
+      <c r="W130">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="131" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U131" t="s">
+        <v>437</v>
+      </c>
+      <c r="V131" t="s">
+        <v>438</v>
+      </c>
+      <c r="W131">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="132" spans="21:23" x14ac:dyDescent="0.3">
+      <c r="U132" t="s">
+        <v>439</v>
+      </c>
+      <c r="V132" t="s">
+        <v>440</v>
+      </c>
+      <c r="W132">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="L1:O1"/>
+    <mergeCell ref="A27:I27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1448,7 +3746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6099AB90-333A-4163-8EBA-AEC90724930B}">
   <dimension ref="B1:V2257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+    <sheetView topLeftCell="B3" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>

</xml_diff>